<commit_message>
Query RDF sobre inmuebles
</commit_message>
<xml_diff>
--- a/PropiedadesInfocasas.xlsx
+++ b/PropiedadesInfocasas.xlsx
@@ -70,10 +70,10 @@
     <t xml:space="preserve">Palermo</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 1</t>
+    <t xml:space="preserve">Infocasas – Publicación 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 1</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
@@ -94,10 +94,10 @@
     <t xml:space="preserve">Buceo</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 2</t>
+    <t xml:space="preserve">Infocasas – Publicación 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 2</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
@@ -118,10 +118,10 @@
     <t xml:space="preserve">Carrasco</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 3</t>
+    <t xml:space="preserve">Infocasas – Publicación 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 3</t>
   </si>
   <si>
     <t xml:space="preserve">House</t>
@@ -145,10 +145,10 @@
     <t xml:space="preserve">Parque Rodó</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 4</t>
+    <t xml:space="preserve">Infocasas – Publicación 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 4</t>
   </si>
   <si>
     <t xml:space="preserve">Herrera y Reissig</t>
@@ -166,10 +166,10 @@
     <t xml:space="preserve">Pocitos</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 5</t>
+    <t xml:space="preserve">Infocasas – Publicación 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 5</t>
   </si>
   <si>
     <t xml:space="preserve">4</t>
@@ -184,10 +184,10 @@
     <t xml:space="preserve">29024325</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 6</t>
+    <t xml:space="preserve">Infocasas – Publicación 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 6</t>
   </si>
   <si>
     <t xml:space="preserve">Rizal</t>
@@ -202,10 +202,10 @@
     <t xml:space="preserve">29024326</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 7</t>
+    <t xml:space="preserve">Infocasas – Publicación 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 7</t>
   </si>
   <si>
     <t xml:space="preserve">Isla de Flores</t>
@@ -223,10 +223,10 @@
     <t xml:space="preserve">Cordón</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 8</t>
+    <t xml:space="preserve">Infocasas – Publicación 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 8</t>
   </si>
   <si>
     <t xml:space="preserve">Colonia</t>
@@ -241,10 +241,10 @@
     <t xml:space="preserve">Parque Batlle</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 9</t>
+    <t xml:space="preserve">Infocasas – Publicación 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 9</t>
   </si>
   <si>
     <t xml:space="preserve">Ponce</t>
@@ -256,10 +256,10 @@
     <t xml:space="preserve">Centro</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 10</t>
+    <t xml:space="preserve">Infocasas – Publicación 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 10</t>
   </si>
   <si>
     <t xml:space="preserve">Santiago de Chile</t>
@@ -277,10 +277,10 @@
     <t xml:space="preserve">Punta Gorda</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 11</t>
+    <t xml:space="preserve">Infocasas – Publicación 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 11</t>
   </si>
   <si>
     <t xml:space="preserve">Caramuru</t>
@@ -295,10 +295,10 @@
     <t xml:space="preserve">Malvín</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 12</t>
+    <t xml:space="preserve">Infocasas – Publicación 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 12</t>
   </si>
   <si>
     <t xml:space="preserve">Pilcomayo</t>
@@ -313,19 +313,19 @@
     <t xml:space="preserve">29024332</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 13</t>
+    <t xml:space="preserve">Infocasas – Publicación 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 13</t>
   </si>
   <si>
     <t xml:space="preserve">Tristnán Narvaja</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 14</t>
+    <t xml:space="preserve">Infocasas – Publicación 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 14</t>
   </si>
   <si>
     <t xml:space="preserve">Fernández Crespo</t>
@@ -343,10 +343,10 @@
     <t xml:space="preserve">Peñarol</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 15</t>
+    <t xml:space="preserve">Infocasas – Publicación 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 15</t>
   </si>
   <si>
     <t xml:space="preserve">Camino Coronel Raíz</t>
@@ -364,10 +364,10 @@
     <t xml:space="preserve">Aguada</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 16</t>
+    <t xml:space="preserve">Infocasas – Publicación 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 16</t>
   </si>
   <si>
     <t xml:space="preserve">Nueva York</t>
@@ -379,10 +379,10 @@
     <t xml:space="preserve">29024336</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 17</t>
+    <t xml:space="preserve">Infocasas – Publicación 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 17</t>
   </si>
   <si>
     <t xml:space="preserve">Soca</t>
@@ -394,10 +394,10 @@
     <t xml:space="preserve">29024337</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 18</t>
+    <t xml:space="preserve">Infocasas – Publicación 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 18</t>
   </si>
   <si>
     <t xml:space="preserve">Ramón Anador</t>
@@ -409,10 +409,10 @@
     <t xml:space="preserve">29024338</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 19</t>
+    <t xml:space="preserve">Infocasas – Publicación 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 19</t>
   </si>
   <si>
     <t xml:space="preserve">Av Brasil</t>
@@ -427,10 +427,10 @@
     <t xml:space="preserve">29024339</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 20</t>
+    <t xml:space="preserve">Infocasas – Publicación 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 20</t>
   </si>
   <si>
     <t xml:space="preserve">Rivera</t>
@@ -445,10 +445,10 @@
     <t xml:space="preserve">29024340</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 21</t>
+    <t xml:space="preserve">Infocasas – Publicación 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 21</t>
   </si>
   <si>
     <t xml:space="preserve">Rimac</t>
@@ -463,10 +463,10 @@
     <t xml:space="preserve">Ciudad Vieja</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 22</t>
+    <t xml:space="preserve">Infocasas – Publicación 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 22</t>
   </si>
   <si>
     <t xml:space="preserve">Treinta y tres</t>
@@ -566,7 +566,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -580,10 +580,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -610,18 +606,19 @@
   </sheetPr>
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="L24" activeCellId="0" sqref="L24"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.43"/>
@@ -744,7 +741,7 @@
       <c r="C3" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="0" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -815,10 +812,10 @@
       <c r="K4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M4" s="5" t="n">
+      <c r="M4" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N4" s="3" t="s">
@@ -879,13 +876,13 @@
       <c r="A6" s="3" t="n">
         <v>52000</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="0" t="s">
         <v>49</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -909,10 +906,10 @@
       <c r="K6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="5" t="n">
+      <c r="M6" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N6" s="3" t="s">
@@ -926,7 +923,7 @@
       <c r="A7" s="3" t="n">
         <v>38000</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="0" t="s">
@@ -1012,7 +1009,7 @@
       <c r="N8" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="O8" s="5" t="s">
+      <c r="O8" s="4" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1026,7 +1023,7 @@
       <c r="C9" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="0" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1050,10 +1047,10 @@
       <c r="K9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="5" t="n">
+      <c r="M9" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N9" s="3" t="s">
@@ -1067,7 +1064,7 @@
       <c r="A10" s="3" t="n">
         <v>27000</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C10" s="0" t="s">
@@ -1091,7 +1088,7 @@
       <c r="I10" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="4" t="s">
         <v>75</v>
       </c>
       <c r="K10" s="3" t="s">
@@ -1103,10 +1100,10 @@
       <c r="M10" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="O10" s="5" t="s">
+      <c r="O10" s="4" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1144,7 +1141,7 @@
       <c r="K11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="L11" s="4" t="s">
         <v>81</v>
       </c>
       <c r="M11" s="3" t="n">
@@ -1158,7 +1155,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
+      <c r="A12" s="4" t="n">
         <v>75000</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1167,7 +1164,7 @@
       <c r="C12" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="0" t="s">
         <v>86</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1191,10 +1188,10 @@
       <c r="K12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="5" t="n">
+      <c r="M12" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N12" s="3" t="s">
@@ -1294,7 +1291,7 @@
       <c r="N14" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="O14" s="5" t="s">
+      <c r="O14" s="4" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1308,7 +1305,7 @@
       <c r="C15" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="0" t="s">
         <v>101</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1426,10 +1423,10 @@
       <c r="K17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="L17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M17" s="5" t="n">
+      <c r="M17" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N17" s="3" t="s">
@@ -1449,7 +1446,7 @@
       <c r="C18" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="0" t="s">
         <v>120</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -1473,10 +1470,10 @@
       <c r="K18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="L18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M18" s="5" t="n">
+      <c r="M18" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N18" s="3" t="s">
@@ -1537,7 +1534,7 @@
       <c r="A20" s="3" t="n">
         <v>29500</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C20" s="0" t="s">
@@ -1573,7 +1570,7 @@
       <c r="M20" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="N20" s="5" t="s">
+      <c r="N20" s="4" t="s">
         <v>133</v>
       </c>
       <c r="O20" s="3" t="s">
@@ -1590,7 +1587,7 @@
       <c r="C21" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="0" t="s">
         <v>136</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -1661,10 +1658,10 @@
       <c r="K22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="L22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M22" s="5" t="n">
+      <c r="M22" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N22" s="3" t="s">
@@ -1702,7 +1699,7 @@
       <c r="I23" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J23" s="4" t="s">
         <v>149</v>
       </c>
       <c r="K23" s="3" t="s">

</xml_diff>

<commit_message>
Query RDF sobre inmuebles (#8)
Query RDF sobre inmuebles
Query RDF sobre anep
</commit_message>
<xml_diff>
--- a/PropiedadesInfocasas.xlsx
+++ b/PropiedadesInfocasas.xlsx
@@ -70,10 +70,10 @@
     <t xml:space="preserve">Palermo</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 1</t>
+    <t xml:space="preserve">Infocasas – Publicación 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 1</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
@@ -94,10 +94,10 @@
     <t xml:space="preserve">Buceo</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 2</t>
+    <t xml:space="preserve">Infocasas – Publicación 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 2</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
@@ -118,10 +118,10 @@
     <t xml:space="preserve">Carrasco</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 3</t>
+    <t xml:space="preserve">Infocasas – Publicación 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 3</t>
   </si>
   <si>
     <t xml:space="preserve">House</t>
@@ -145,10 +145,10 @@
     <t xml:space="preserve">Parque Rodó</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 4</t>
+    <t xml:space="preserve">Infocasas – Publicación 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 4</t>
   </si>
   <si>
     <t xml:space="preserve">Herrera y Reissig</t>
@@ -166,10 +166,10 @@
     <t xml:space="preserve">Pocitos</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 5</t>
+    <t xml:space="preserve">Infocasas – Publicación 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 5</t>
   </si>
   <si>
     <t xml:space="preserve">4</t>
@@ -184,10 +184,10 @@
     <t xml:space="preserve">29024325</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 6</t>
+    <t xml:space="preserve">Infocasas – Publicación 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 6</t>
   </si>
   <si>
     <t xml:space="preserve">Rizal</t>
@@ -202,10 +202,10 @@
     <t xml:space="preserve">29024326</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 7</t>
+    <t xml:space="preserve">Infocasas – Publicación 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 7</t>
   </si>
   <si>
     <t xml:space="preserve">Isla de Flores</t>
@@ -223,10 +223,10 @@
     <t xml:space="preserve">Cordón</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 8</t>
+    <t xml:space="preserve">Infocasas – Publicación 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 8</t>
   </si>
   <si>
     <t xml:space="preserve">Colonia</t>
@@ -241,10 +241,10 @@
     <t xml:space="preserve">Parque Batlle</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 9</t>
+    <t xml:space="preserve">Infocasas – Publicación 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 9</t>
   </si>
   <si>
     <t xml:space="preserve">Ponce</t>
@@ -256,10 +256,10 @@
     <t xml:space="preserve">Centro</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 10</t>
+    <t xml:space="preserve">Infocasas – Publicación 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 10</t>
   </si>
   <si>
     <t xml:space="preserve">Santiago de Chile</t>
@@ -277,10 +277,10 @@
     <t xml:space="preserve">Punta Gorda</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 11</t>
+    <t xml:space="preserve">Infocasas – Publicación 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 11</t>
   </si>
   <si>
     <t xml:space="preserve">Caramuru</t>
@@ -295,10 +295,10 @@
     <t xml:space="preserve">Malvín</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 12</t>
+    <t xml:space="preserve">Infocasas – Publicación 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 12</t>
   </si>
   <si>
     <t xml:space="preserve">Pilcomayo</t>
@@ -313,19 +313,19 @@
     <t xml:space="preserve">29024332</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 13</t>
+    <t xml:space="preserve">Infocasas – Publicación 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 13</t>
   </si>
   <si>
     <t xml:space="preserve">Tristnán Narvaja</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 14</t>
+    <t xml:space="preserve">Infocasas – Publicación 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 14</t>
   </si>
   <si>
     <t xml:space="preserve">Fernández Crespo</t>
@@ -343,10 +343,10 @@
     <t xml:space="preserve">Peñarol</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 15</t>
+    <t xml:space="preserve">Infocasas – Publicación 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 15</t>
   </si>
   <si>
     <t xml:space="preserve">Camino Coronel Raíz</t>
@@ -364,10 +364,10 @@
     <t xml:space="preserve">Aguada</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 16</t>
+    <t xml:space="preserve">Infocasas – Publicación 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 16</t>
   </si>
   <si>
     <t xml:space="preserve">Nueva York</t>
@@ -379,10 +379,10 @@
     <t xml:space="preserve">29024336</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 17</t>
+    <t xml:space="preserve">Infocasas – Publicación 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 17</t>
   </si>
   <si>
     <t xml:space="preserve">Soca</t>
@@ -394,10 +394,10 @@
     <t xml:space="preserve">29024337</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 18</t>
+    <t xml:space="preserve">Infocasas – Publicación 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 18</t>
   </si>
   <si>
     <t xml:space="preserve">Ramón Anador</t>
@@ -409,10 +409,10 @@
     <t xml:space="preserve">29024338</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 19</t>
+    <t xml:space="preserve">Infocasas – Publicación 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 19</t>
   </si>
   <si>
     <t xml:space="preserve">Av Brasil</t>
@@ -427,10 +427,10 @@
     <t xml:space="preserve">29024339</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 20</t>
+    <t xml:space="preserve">Infocasas – Publicación 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 20</t>
   </si>
   <si>
     <t xml:space="preserve">Rivera</t>
@@ -445,10 +445,10 @@
     <t xml:space="preserve">29024340</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 21</t>
+    <t xml:space="preserve">Infocasas – Publicación 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 21</t>
   </si>
   <si>
     <t xml:space="preserve">Rimac</t>
@@ -463,10 +463,10 @@
     <t xml:space="preserve">Ciudad Vieja</t>
   </si>
   <si>
-    <t xml:space="preserve">Publicación 22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de publicación 22</t>
+    <t xml:space="preserve">Infocasas – Publicación 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infocasas – Descripción 22</t>
   </si>
   <si>
     <t xml:space="preserve">Treinta y tres</t>
@@ -566,7 +566,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -580,10 +580,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -610,18 +606,19 @@
   </sheetPr>
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="L24" activeCellId="0" sqref="L24"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.43"/>
@@ -744,7 +741,7 @@
       <c r="C3" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="0" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -815,10 +812,10 @@
       <c r="K4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M4" s="5" t="n">
+      <c r="M4" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N4" s="3" t="s">
@@ -879,13 +876,13 @@
       <c r="A6" s="3" t="n">
         <v>52000</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="0" t="s">
         <v>49</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -909,10 +906,10 @@
       <c r="K6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="5" t="n">
+      <c r="M6" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N6" s="3" t="s">
@@ -926,7 +923,7 @@
       <c r="A7" s="3" t="n">
         <v>38000</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="0" t="s">
@@ -1012,7 +1009,7 @@
       <c r="N8" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="O8" s="5" t="s">
+      <c r="O8" s="4" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1026,7 +1023,7 @@
       <c r="C9" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="0" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1050,10 +1047,10 @@
       <c r="K9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="5" t="n">
+      <c r="M9" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N9" s="3" t="s">
@@ -1067,7 +1064,7 @@
       <c r="A10" s="3" t="n">
         <v>27000</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C10" s="0" t="s">
@@ -1091,7 +1088,7 @@
       <c r="I10" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="4" t="s">
         <v>75</v>
       </c>
       <c r="K10" s="3" t="s">
@@ -1103,10 +1100,10 @@
       <c r="M10" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="O10" s="5" t="s">
+      <c r="O10" s="4" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1144,7 +1141,7 @@
       <c r="K11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="L11" s="4" t="s">
         <v>81</v>
       </c>
       <c r="M11" s="3" t="n">
@@ -1158,7 +1155,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
+      <c r="A12" s="4" t="n">
         <v>75000</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1167,7 +1164,7 @@
       <c r="C12" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="0" t="s">
         <v>86</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1191,10 +1188,10 @@
       <c r="K12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="5" t="n">
+      <c r="M12" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N12" s="3" t="s">
@@ -1294,7 +1291,7 @@
       <c r="N14" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="O14" s="5" t="s">
+      <c r="O14" s="4" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1308,7 +1305,7 @@
       <c r="C15" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="0" t="s">
         <v>101</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1426,10 +1423,10 @@
       <c r="K17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="L17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M17" s="5" t="n">
+      <c r="M17" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N17" s="3" t="s">
@@ -1449,7 +1446,7 @@
       <c r="C18" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="0" t="s">
         <v>120</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -1473,10 +1470,10 @@
       <c r="K18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="L18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M18" s="5" t="n">
+      <c r="M18" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N18" s="3" t="s">
@@ -1537,7 +1534,7 @@
       <c r="A20" s="3" t="n">
         <v>29500</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C20" s="0" t="s">
@@ -1573,7 +1570,7 @@
       <c r="M20" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="N20" s="5" t="s">
+      <c r="N20" s="4" t="s">
         <v>133</v>
       </c>
       <c r="O20" s="3" t="s">
@@ -1590,7 +1587,7 @@
       <c r="C21" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="0" t="s">
         <v>136</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -1661,10 +1658,10 @@
       <c r="K22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="L22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M22" s="5" t="n">
+      <c r="M22" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N22" s="3" t="s">
@@ -1702,7 +1699,7 @@
       <c r="I23" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J23" s="4" t="s">
         <v>149</v>
       </c>
       <c r="K23" s="3" t="s">

</xml_diff>